<commit_message>
PCB rev2-230718 Update to Use throughhole audio jacks (C2939180)
</commit_message>
<xml_diff>
--- a/rev2/aqplus_rev2_BOM.xlsx
+++ b/rev2/aqplus_rev2_BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sph\Box\Retro\Aquarius\Aquarius Plus\aquarius-plus\pcb\rev2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sph\Box\Retro\Aquarius\AquariusPlus\aquarius-plus\System\pcb\rev2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A14AFA-379A-4814-9A2B-955724849332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA1D1802-DEA0-4117-A1E9-DD4B12D7E614}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11295" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -570,9 +570,6 @@
     <t>C138387</t>
   </si>
   <si>
-    <t>C2884998</t>
-  </si>
-  <si>
     <t>PJ-320B-SMT</t>
   </si>
   <si>
@@ -580,6 +577,9 @@
   </si>
   <si>
     <t>C7431259</t>
+  </si>
+  <si>
+    <t>C2939180</t>
   </si>
 </sst>
 </file>
@@ -1046,8 +1046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -1114,7 +1114,7 @@
         <v>124</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E4" s="7"/>
     </row>
@@ -1368,10 +1368,10 @@
         <v>75</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15">
@@ -1536,10 +1536,10 @@
         <v>86</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15">
@@ -1718,10 +1718,10 @@
         <v>99</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="57">
@@ -1749,7 +1749,7 @@
         <v>122</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15">
@@ -1774,10 +1774,10 @@
         <v>103</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>